<commit_message>
Push with Nicco Analysis
</commit_message>
<xml_diff>
--- a/Nicco Tags Analysis.xlsx
+++ b/Nicco Tags Analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="229">
   <si>
     <t>Nicco</t>
   </si>
@@ -701,6 +701,12 @@
   </si>
   <si>
     <t>Most errors are caused by verbs</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy </t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,9 +2544,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80">
+        <f>SUM(D2:D79)</f>
+        <v>53</v>
+      </c>
+      <c r="E80">
+        <f>SUM(E2:E79)</f>
+        <v>269</v>
+      </c>
+      <c r="F80">
+        <f t="shared" ref="F80:G80" si="0">SUM(F2:F79)</f>
+        <v>18</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82">
+        <f>1-(D80/E80)</f>
+        <v>0.80297397769516732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>